<commit_message>
meer gui nog een probleem met checkmate
</commit_message>
<xml_diff>
--- a/schaken.xlsx
+++ b/schaken.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RafaelDeSmet\Dropbox\MasterInformatica\Schaken\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24FCD7FC-67CC-4E2A-A489-973B9435C430}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9370D41-BE78-4A83-BE9F-1B55D6D00676}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AD0A2C39-4502-4769-AC27-39808CD06FAC}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="96">
   <si>
     <t>PAWN</t>
   </si>
@@ -232,6 +232,93 @@
   </si>
   <si>
     <t>King</t>
+  </si>
+  <si>
+    <t>wit:</t>
+  </si>
+  <si>
+    <t>grijs:</t>
+  </si>
+  <si>
+    <t>r=0,c=1</t>
+  </si>
+  <si>
+    <t>r=0,c=4</t>
+  </si>
+  <si>
+    <t>r=0,c=5</t>
+  </si>
+  <si>
+    <t>r=0,c=6</t>
+  </si>
+  <si>
+    <t>r=0,c=7</t>
+  </si>
+  <si>
+    <t>r=1,c=2</t>
+  </si>
+  <si>
+    <t>r=1,c=4</t>
+  </si>
+  <si>
+    <t>r=1,c=5</t>
+  </si>
+  <si>
+    <t>r=1,c=6</t>
+  </si>
+  <si>
+    <t>r=1,c=7</t>
+  </si>
+  <si>
+    <t>r=3,c=1</t>
+  </si>
+  <si>
+    <t>r=2,c=6</t>
+  </si>
+  <si>
+    <t>r=3,c=2</t>
+  </si>
+  <si>
+    <t>r=3,c=4</t>
+  </si>
+  <si>
+    <t>r=4,c=1</t>
+  </si>
+  <si>
+    <t>r=4,c=2</t>
+  </si>
+  <si>
+    <t>r=4,c=4</t>
+  </si>
+  <si>
+    <t>r=5,c=6</t>
+  </si>
+  <si>
+    <t>r=6,c=2</t>
+  </si>
+  <si>
+    <t>r=6,c=4</t>
+  </si>
+  <si>
+    <t>r=6,c=5</t>
+  </si>
+  <si>
+    <t>r=6,c=6</t>
+  </si>
+  <si>
+    <t>r=6,c=7</t>
+  </si>
+  <si>
+    <t>r=7,c=4</t>
+  </si>
+  <si>
+    <t>r=7,c=5</t>
+  </si>
+  <si>
+    <t>r=7,c=6</t>
+  </si>
+  <si>
+    <t>r=7,c=7</t>
   </si>
 </sst>
 </file>
@@ -868,7 +955,7 @@
   <dimension ref="A4:X67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1117,6 +1204,21 @@
       <c r="D16" s="17" t="s">
         <v>61</v>
       </c>
+      <c r="F16" t="s">
+        <v>67</v>
+      </c>
+      <c r="G16" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" t="s">
+        <v>37</v>
+      </c>
+      <c r="I16" t="s">
+        <v>70</v>
+      </c>
+      <c r="J16" t="s">
+        <v>72</v>
+      </c>
       <c r="L16" s="9"/>
       <c r="O16" s="11" t="s">
         <v>28</v>
@@ -1136,6 +1238,18 @@
       <c r="D17" s="20" t="s">
         <v>61</v>
       </c>
+      <c r="G17" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17" t="s">
+        <v>76</v>
+      </c>
+      <c r="J17" t="s">
+        <v>78</v>
+      </c>
       <c r="L17" s="9" t="s">
         <v>15</v>
       </c>
@@ -1163,6 +1277,18 @@
       <c r="D18" s="20" t="s">
         <v>61</v>
       </c>
+      <c r="G18" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I18" t="s">
+        <v>39</v>
+      </c>
+      <c r="J18" t="s">
+        <v>80</v>
+      </c>
       <c r="O18" s="11" t="s">
         <v>28</v>
       </c>
@@ -1181,6 +1307,18 @@
       <c r="D19" s="20" t="s">
         <v>61</v>
       </c>
+      <c r="G19" t="s">
+        <v>79</v>
+      </c>
+      <c r="H19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" t="s">
+        <v>40</v>
+      </c>
+      <c r="J19" t="s">
+        <v>58</v>
+      </c>
       <c r="L19" s="9" t="s">
         <v>30</v>
       </c>
@@ -1220,6 +1358,18 @@
       <c r="D20" s="20" t="s">
         <v>61</v>
       </c>
+      <c r="G20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" t="s">
+        <v>84</v>
+      </c>
+      <c r="I20" t="s">
+        <v>85</v>
+      </c>
+      <c r="J20" t="s">
+        <v>41</v>
+      </c>
       <c r="O20" s="11" t="s">
         <v>28</v>
       </c>
@@ -1250,6 +1400,18 @@
       <c r="D21" s="20" t="s">
         <v>61</v>
       </c>
+      <c r="G21" t="s">
+        <v>59</v>
+      </c>
+      <c r="H21" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" t="s">
+        <v>51</v>
+      </c>
+      <c r="J21" t="s">
+        <v>42</v>
+      </c>
       <c r="L21" s="9" t="s">
         <v>18</v>
       </c>
@@ -1289,6 +1451,18 @@
       <c r="D22" s="17" t="s">
         <v>63</v>
       </c>
+      <c r="G22" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" t="s">
+        <v>87</v>
+      </c>
+      <c r="I22" t="s">
+        <v>88</v>
+      </c>
+      <c r="J22" t="s">
+        <v>90</v>
+      </c>
       <c r="O22" s="11" t="s">
         <v>28</v>
       </c>
@@ -1319,6 +1493,18 @@
       <c r="D23" s="20" t="s">
         <v>63</v>
       </c>
+      <c r="G23" t="s">
+        <v>34</v>
+      </c>
+      <c r="H23" t="s">
+        <v>57</v>
+      </c>
+      <c r="I23" t="s">
+        <v>93</v>
+      </c>
+      <c r="J23" t="s">
+        <v>95</v>
+      </c>
       <c r="L23" s="9" t="s">
         <v>31</v>
       </c>
@@ -1358,6 +1544,21 @@
       <c r="D25" s="20" t="s">
         <v>63</v>
       </c>
+      <c r="F25" t="s">
+        <v>68</v>
+      </c>
+      <c r="G25" t="s">
+        <v>69</v>
+      </c>
+      <c r="H25" t="s">
+        <v>50</v>
+      </c>
+      <c r="I25" t="s">
+        <v>71</v>
+      </c>
+      <c r="J25" t="s">
+        <v>73</v>
+      </c>
       <c r="L25" s="9" t="s">
         <v>33</v>
       </c>
@@ -1382,6 +1583,18 @@
       <c r="D26" s="20" t="s">
         <v>63</v>
       </c>
+      <c r="G26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H26" t="s">
+        <v>74</v>
+      </c>
+      <c r="I26" t="s">
+        <v>75</v>
+      </c>
+      <c r="J26" t="s">
+        <v>77</v>
+      </c>
       <c r="O26" s="11" t="s">
         <v>28</v>
       </c>
@@ -1397,6 +1610,18 @@
       <c r="D27" s="20" t="s">
         <v>63</v>
       </c>
+      <c r="G27" t="s">
+        <v>54</v>
+      </c>
+      <c r="H27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" t="s">
+        <v>52</v>
+      </c>
+      <c r="J27" t="s">
+        <v>48</v>
+      </c>
       <c r="L27" s="9" t="s">
         <v>36</v>
       </c>
@@ -1438,7 +1663,18 @@
       </c>
       <c r="E28" s="14"/>
       <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
+      <c r="G28" t="s">
+        <v>24</v>
+      </c>
+      <c r="H28" t="s">
+        <v>81</v>
+      </c>
+      <c r="I28" t="s">
+        <v>82</v>
+      </c>
+      <c r="J28" t="s">
+        <v>47</v>
+      </c>
       <c r="O28" s="11" t="s">
         <v>28</v>
       </c>
@@ -1471,7 +1707,18 @@
       </c>
       <c r="E29" s="14"/>
       <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
+      <c r="G29" t="s">
+        <v>83</v>
+      </c>
+      <c r="H29" t="s">
+        <v>12</v>
+      </c>
+      <c r="I29" t="s">
+        <v>46</v>
+      </c>
+      <c r="J29" t="s">
+        <v>53</v>
+      </c>
       <c r="L29" s="9" t="s">
         <v>43</v>
       </c>
@@ -1513,7 +1760,18 @@
       </c>
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
+      <c r="G30" t="s">
+        <v>22</v>
+      </c>
+      <c r="H30" t="s">
+        <v>35</v>
+      </c>
+      <c r="I30" t="s">
+        <v>45</v>
+      </c>
+      <c r="J30" t="s">
+        <v>86</v>
+      </c>
       <c r="O30" s="11" t="s">
         <v>28</v>
       </c>
@@ -1546,7 +1804,18 @@
       </c>
       <c r="E31" s="14"/>
       <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
+      <c r="G31" t="s">
+        <v>21</v>
+      </c>
+      <c r="H31" t="s">
+        <v>16</v>
+      </c>
+      <c r="I31" t="s">
+        <v>89</v>
+      </c>
+      <c r="J31" t="s">
+        <v>91</v>
+      </c>
       <c r="L31" s="9" t="s">
         <v>49</v>
       </c>
@@ -1594,7 +1863,18 @@
       </c>
       <c r="E32" s="14"/>
       <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
+      <c r="G32" t="s">
+        <v>19</v>
+      </c>
+      <c r="H32" t="s">
+        <v>44</v>
+      </c>
+      <c r="I32" t="s">
+        <v>92</v>
+      </c>
+      <c r="J32" t="s">
+        <v>94</v>
+      </c>
       <c r="O32" s="11" t="s">
         <v>28</v>
       </c>
@@ -1677,8 +1957,21 @@
         <v>65</v>
       </c>
       <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
+      <c r="F34" t="s">
+        <v>67</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>2</v>
+      </c>
+      <c r="I34">
+        <v>4</v>
+      </c>
+      <c r="J34">
+        <v>6</v>
+      </c>
       <c r="O34" s="11" t="s">
         <v>28</v>
       </c>
@@ -1716,8 +2009,18 @@
         <v>65</v>
       </c>
       <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
+      <c r="G35">
+        <v>2</v>
+      </c>
+      <c r="H35">
+        <v>4</v>
+      </c>
+      <c r="I35">
+        <v>6</v>
+      </c>
+      <c r="J35">
+        <v>8</v>
+      </c>
     </row>
     <row r="36" spans="2:24" x14ac:dyDescent="0.55000000000000004">
       <c r="B36" s="18" t="s">
@@ -1728,8 +2031,18 @@
         <v>65</v>
       </c>
       <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
+      <c r="G36">
+        <v>2</v>
+      </c>
+      <c r="H36">
+        <v>4</v>
+      </c>
+      <c r="I36">
+        <v>6</v>
+      </c>
+      <c r="J36">
+        <v>8</v>
+      </c>
     </row>
     <row r="37" spans="2:24" x14ac:dyDescent="0.55000000000000004">
       <c r="B37" s="18" t="s">
@@ -1740,8 +2053,18 @@
         <v>65</v>
       </c>
       <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
+      <c r="G37">
+        <v>4</v>
+      </c>
+      <c r="H37">
+        <v>6</v>
+      </c>
+      <c r="I37">
+        <v>8</v>
+      </c>
+      <c r="J37">
+        <v>10</v>
+      </c>
     </row>
     <row r="38" spans="2:24" x14ac:dyDescent="0.55000000000000004">
       <c r="B38" s="18" t="s">
@@ -1752,8 +2075,18 @@
         <v>65</v>
       </c>
       <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
+      <c r="G38">
+        <v>4</v>
+      </c>
+      <c r="H38">
+        <v>6</v>
+      </c>
+      <c r="I38">
+        <v>8</v>
+      </c>
+      <c r="J38">
+        <v>10</v>
+      </c>
     </row>
     <row r="39" spans="2:24" x14ac:dyDescent="0.55000000000000004">
       <c r="B39" s="21" t="s">
@@ -1763,6 +2096,18 @@
       <c r="D39" s="23" t="s">
         <v>65</v>
       </c>
+      <c r="G39">
+        <v>6</v>
+      </c>
+      <c r="H39">
+        <v>8</v>
+      </c>
+      <c r="I39">
+        <v>10</v>
+      </c>
+      <c r="J39">
+        <v>12</v>
+      </c>
     </row>
     <row r="40" spans="2:24" x14ac:dyDescent="0.55000000000000004">
       <c r="B40" s="15" t="s">
@@ -1773,8 +2118,18 @@
         <v>60</v>
       </c>
       <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
+      <c r="G40">
+        <v>6</v>
+      </c>
+      <c r="H40">
+        <v>8</v>
+      </c>
+      <c r="I40">
+        <v>10</v>
+      </c>
+      <c r="J40">
+        <v>12</v>
+      </c>
     </row>
     <row r="41" spans="2:24" x14ac:dyDescent="0.55000000000000004">
       <c r="B41" s="18" t="s">
@@ -1785,8 +2140,18 @@
         <v>60</v>
       </c>
       <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
+      <c r="G41">
+        <v>8</v>
+      </c>
+      <c r="H41">
+        <v>10</v>
+      </c>
+      <c r="I41">
+        <v>12</v>
+      </c>
+      <c r="J41">
+        <v>14</v>
+      </c>
     </row>
     <row r="42" spans="2:24" x14ac:dyDescent="0.55000000000000004">
       <c r="B42" s="18" t="s">
@@ -1797,8 +2162,6 @@
         <v>60</v>
       </c>
       <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
     </row>
     <row r="43" spans="2:24" x14ac:dyDescent="0.55000000000000004">
       <c r="B43" s="18" t="s">
@@ -1809,8 +2172,21 @@
         <v>60</v>
       </c>
       <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
+      <c r="F43" t="s">
+        <v>68</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43">
+        <v>3</v>
+      </c>
+      <c r="I43">
+        <v>5</v>
+      </c>
+      <c r="J43">
+        <v>7</v>
+      </c>
     </row>
     <row r="44" spans="2:24" x14ac:dyDescent="0.55000000000000004">
       <c r="B44" s="18" t="s">
@@ -1821,8 +2197,18 @@
         <v>60</v>
       </c>
       <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44">
+        <v>3</v>
+      </c>
+      <c r="I44">
+        <v>5</v>
+      </c>
+      <c r="J44">
+        <v>6</v>
+      </c>
     </row>
     <row r="45" spans="2:24" x14ac:dyDescent="0.55000000000000004">
       <c r="B45" s="21" t="s">
@@ -1832,6 +2218,18 @@
       <c r="D45" s="23" t="s">
         <v>60</v>
       </c>
+      <c r="G45">
+        <v>3</v>
+      </c>
+      <c r="H45">
+        <v>5</v>
+      </c>
+      <c r="I45">
+        <v>7</v>
+      </c>
+      <c r="J45">
+        <v>9</v>
+      </c>
     </row>
     <row r="46" spans="2:24" x14ac:dyDescent="0.55000000000000004">
       <c r="B46" s="15" t="s">
@@ -1843,7 +2241,18 @@
       </c>
       <c r="E46" s="14"/>
       <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
+      <c r="G46">
+        <v>3</v>
+      </c>
+      <c r="H46">
+        <v>5</v>
+      </c>
+      <c r="I46">
+        <v>7</v>
+      </c>
+      <c r="J46">
+        <v>9</v>
+      </c>
     </row>
     <row r="47" spans="2:24" x14ac:dyDescent="0.55000000000000004">
       <c r="B47" s="18" t="s">
@@ -1855,7 +2264,18 @@
       </c>
       <c r="E47" s="14"/>
       <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
+      <c r="G47">
+        <v>5</v>
+      </c>
+      <c r="H47">
+        <v>7</v>
+      </c>
+      <c r="I47">
+        <v>9</v>
+      </c>
+      <c r="J47">
+        <v>11</v>
+      </c>
     </row>
     <row r="48" spans="2:24" x14ac:dyDescent="0.55000000000000004">
       <c r="B48" s="18" t="s">
@@ -1867,7 +2287,18 @@
       </c>
       <c r="E48" s="14"/>
       <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
+      <c r="G48">
+        <v>5</v>
+      </c>
+      <c r="H48">
+        <v>7</v>
+      </c>
+      <c r="I48">
+        <v>9</v>
+      </c>
+      <c r="J48">
+        <v>11</v>
+      </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B49" s="18" t="s">
@@ -1879,7 +2310,18 @@
       </c>
       <c r="E49" s="14"/>
       <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="G49">
+        <v>7</v>
+      </c>
+      <c r="H49">
+        <v>9</v>
+      </c>
+      <c r="I49">
+        <v>11</v>
+      </c>
+      <c r="J49">
+        <v>13</v>
+      </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B50" s="18" t="s">
@@ -1891,7 +2333,18 @@
       </c>
       <c r="E50" s="14"/>
       <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="G50">
+        <v>7</v>
+      </c>
+      <c r="H50">
+        <v>9</v>
+      </c>
+      <c r="I50">
+        <v>11</v>
+      </c>
+      <c r="J50">
+        <v>13</v>
+      </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B51" s="21" t="s">

</xml_diff>

<commit_message>
todo ga over possibleMoves/getLegal/takeable
</commit_message>
<xml_diff>
--- a/schaken.xlsx
+++ b/schaken.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RafaelDeSmet\Dropbox\MasterInformatica\Schaken\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9370D41-BE78-4A83-BE9F-1B55D6D00676}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CB3D7E-14D1-4847-A2DE-A585A8C5FA3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AD0A2C39-4502-4769-AC27-39808CD06FAC}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="96">
   <si>
     <t>PAWN</t>
   </si>
@@ -377,7 +377,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -423,6 +423,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -596,7 +602,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -633,6 +639,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="60% - Accent1" xfId="5" builtinId="32"/>
@@ -955,7 +964,7 @@
   <dimension ref="A4:X67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -998,59 +1007,29 @@
       <c r="A5" s="5">
         <v>0</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:24" ht="50.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A6" s="5">
         <v>1</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="2"/>
       <c r="F6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="24"/>
     </row>
     <row r="7" spans="1:24" ht="50.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A7" s="5">
@@ -1108,59 +1087,27 @@
       <c r="A11" s="5">
         <v>6</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:24" ht="50.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="5">
         <v>7</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="2"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="M14" s="10" t="s">

</xml_diff>